<commit_message>
Update metadata with depth
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/sinclair/testproj/metadata.xlsx
+++ b/metadata/excel/projects/sinclair/testproj/metadata.xlsx
@@ -16,10 +16,10 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -1889,13 +1889,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="291" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2587,7 +2587,7 @@
     <sheetView tabSelected="1" topLeftCell="BK1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="BT14" sqref="BT14"/>
+      <selection pane="bottomLeft" activeCell="BX2" sqref="BX2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2724,25 +2724,25 @@
       <c r="BC1" s="3"/>
       <c r="BD1" s="3"/>
       <c r="BE1" s="10"/>
-      <c r="BG1" s="65" t="s">
+      <c r="BG1" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="BH1" s="65"/>
-      <c r="BI1" s="65"/>
-      <c r="BJ1" s="65"/>
-      <c r="BL1" s="65" t="s">
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="67"/>
+      <c r="BJ1" s="67"/>
+      <c r="BL1" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="BM1" s="65"/>
-      <c r="BN1" s="65"/>
-      <c r="BO1" s="65"/>
-      <c r="BP1" s="65"/>
-      <c r="BQ1" s="65"/>
-      <c r="BR1" s="65"/>
-      <c r="BT1" s="65" t="s">
+      <c r="BM1" s="67"/>
+      <c r="BN1" s="67"/>
+      <c r="BO1" s="67"/>
+      <c r="BP1" s="67"/>
+      <c r="BQ1" s="67"/>
+      <c r="BR1" s="67"/>
+      <c r="BT1" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="BU1" s="65"/>
+      <c r="BU1" s="67"/>
       <c r="BW1" s="8" t="s">
         <v>68</v>
       </c>
@@ -3700,7 +3700,7 @@
       <c r="BW6">
         <v>10</v>
       </c>
-      <c r="BX6" s="66" t="s">
+      <c r="BX6" s="65" t="s">
         <v>364</v>
       </c>
       <c r="BY6"/>
@@ -3882,7 +3882,7 @@
       <c r="BW7">
         <v>10</v>
       </c>
-      <c r="BX7" s="67" t="s">
+      <c r="BX7" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY7"/>
@@ -4064,7 +4064,7 @@
       <c r="BW8">
         <v>10</v>
       </c>
-      <c r="BX8" s="67" t="s">
+      <c r="BX8" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY8"/>
@@ -4246,7 +4246,7 @@
       <c r="BW9">
         <v>5</v>
       </c>
-      <c r="BX9" s="67" t="s">
+      <c r="BX9" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY9"/>
@@ -4428,7 +4428,7 @@
       <c r="BW10">
         <v>5</v>
       </c>
-      <c r="BX10" s="67" t="s">
+      <c r="BX10" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY10"/>
@@ -4610,7 +4610,7 @@
       <c r="BW11">
         <v>5</v>
       </c>
-      <c r="BX11" s="67" t="s">
+      <c r="BX11" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY11"/>
@@ -4792,7 +4792,7 @@
       <c r="BW12">
         <v>18</v>
       </c>
-      <c r="BX12" s="67" t="s">
+      <c r="BX12" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY12"/>
@@ -4974,7 +4974,7 @@
       <c r="BW13">
         <v>18</v>
       </c>
-      <c r="BX13" s="67" t="s">
+      <c r="BX13" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY13"/>
@@ -5156,7 +5156,7 @@
       <c r="BW14">
         <v>18</v>
       </c>
-      <c r="BX14" s="67" t="s">
+      <c r="BX14" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY14"/>
@@ -5338,7 +5338,7 @@
       <c r="BW15">
         <v>19</v>
       </c>
-      <c r="BX15" s="67" t="s">
+      <c r="BX15" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY15"/>
@@ -5510,7 +5510,7 @@
       <c r="BW16">
         <v>19</v>
       </c>
-      <c r="BX16" s="67" t="s">
+      <c r="BX16" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY16"/>
@@ -5682,7 +5682,7 @@
       <c r="BW17">
         <v>19</v>
       </c>
-      <c r="BX17" s="67" t="s">
+      <c r="BX17" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY17"/>
@@ -5854,7 +5854,7 @@
       <c r="BW18">
         <v>18</v>
       </c>
-      <c r="BX18" s="67" t="s">
+      <c r="BX18" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY18"/>
@@ -6026,7 +6026,7 @@
       <c r="BW19">
         <v>18</v>
       </c>
-      <c r="BX19" s="67" t="s">
+      <c r="BX19" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY19"/>
@@ -6198,7 +6198,7 @@
       <c r="BW20">
         <v>18</v>
       </c>
-      <c r="BX20" s="67" t="s">
+      <c r="BX20" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY20"/>
@@ -6886,7 +6886,7 @@
       <c r="BW24">
         <v>5.5</v>
       </c>
-      <c r="BX24" s="67" t="s">
+      <c r="BX24" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY24"/>
@@ -7058,7 +7058,7 @@
       <c r="BW25">
         <v>5.5</v>
       </c>
-      <c r="BX25" s="67" t="s">
+      <c r="BX25" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY25"/>
@@ -7230,7 +7230,7 @@
       <c r="BW26">
         <v>5.5</v>
       </c>
-      <c r="BX26" s="67" t="s">
+      <c r="BX26" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY26"/>
@@ -7402,7 +7402,7 @@
       <c r="BW27">
         <v>6.5</v>
       </c>
-      <c r="BX27" s="67" t="s">
+      <c r="BX27" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY27"/>
@@ -7574,7 +7574,7 @@
       <c r="BW28">
         <v>6.5</v>
       </c>
-      <c r="BX28" s="67" t="s">
+      <c r="BX28" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY28"/>
@@ -7746,7 +7746,7 @@
       <c r="BW29">
         <v>6.5</v>
       </c>
-      <c r="BX29" s="67" t="s">
+      <c r="BX29" s="66" t="s">
         <v>364</v>
       </c>
       <c r="BY29"/>
@@ -7825,19 +7825,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -7855,14 +7845,24 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Diversity regression plots starting
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/sinclair/testproj/metadata.xlsx
+++ b/metadata/excel/projects/sinclair/testproj/metadata.xlsx
@@ -16,10 +16,10 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="366">
   <si>
     <t>Country</t>
   </si>
@@ -1223,6 +1223,9 @@
   <si>
     <t>MedEx</t>
   </si>
+  <si>
+    <t>Distance to exhaust [m]</t>
+  </si>
 </sst>
 </file>
 
@@ -1231,7 +1234,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1387,8 +1390,15 @@
       <charset val="177"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1449,6 +1459,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDD0806"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1753,7 +1769,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1896,6 +1912,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2582,12 +2604,12 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:CF51"/>
+  <dimension ref="A1:CG51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BK1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="BX2" sqref="BX2"/>
+      <selection pane="bottomLeft" activeCell="BZ7" sqref="BZ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2661,18 +2683,18 @@
     <col min="72" max="72" width="16.5" customWidth="1"/>
     <col min="73" max="73" width="16" customWidth="1"/>
     <col min="74" max="74" width="9.5" customWidth="1"/>
-    <col min="75" max="76" width="11" style="22" customWidth="1"/>
-    <col min="77" max="77" width="11.6640625" style="22" customWidth="1"/>
-    <col min="78" max="78" width="14.33203125" style="22" customWidth="1"/>
-    <col min="79" max="79" width="12.6640625" style="22" customWidth="1"/>
-    <col min="80" max="80" width="13.6640625" style="22" customWidth="1"/>
-    <col min="81" max="81" width="15.33203125" style="22" customWidth="1"/>
-    <col min="82" max="82" width="15.5" style="22" customWidth="1"/>
-    <col min="83" max="83" width="14.6640625" style="22" customWidth="1"/>
-    <col min="84" max="84" width="9.6640625" customWidth="1"/>
+    <col min="75" max="77" width="11" style="22" customWidth="1"/>
+    <col min="78" max="78" width="11.6640625" style="22" customWidth="1"/>
+    <col min="79" max="79" width="14.33203125" style="22" customWidth="1"/>
+    <col min="80" max="80" width="12.6640625" style="22" customWidth="1"/>
+    <col min="81" max="81" width="13.6640625" style="22" customWidth="1"/>
+    <col min="82" max="82" width="15.33203125" style="22" customWidth="1"/>
+    <col min="83" max="83" width="15.5" style="22" customWidth="1"/>
+    <col min="84" max="84" width="14.6640625" style="22" customWidth="1"/>
+    <col min="85" max="85" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
@@ -2747,15 +2769,16 @@
         <v>68</v>
       </c>
       <c r="BX1" s="8"/>
-      <c r="BY1" s="21"/>
+      <c r="BY1" s="8"/>
       <c r="BZ1" s="21"/>
       <c r="CA1" s="21"/>
       <c r="CB1" s="21"/>
       <c r="CC1" s="21"/>
       <c r="CD1" s="21"/>
       <c r="CE1" s="21"/>
+      <c r="CF1" s="21"/>
     </row>
-    <row r="2" spans="1:84" s="52" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:85" s="52" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
         <v>49</v>
       </c>
@@ -2960,30 +2983,33 @@
       <c r="BX2" s="51" t="s">
         <v>362</v>
       </c>
-      <c r="BY2" s="51" t="s">
+      <c r="BY2" s="68" t="s">
+        <v>365</v>
+      </c>
+      <c r="BZ2" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="BZ2" s="51" t="s">
+      <c r="CA2" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="CA2" s="51" t="s">
+      <c r="CB2" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="CB2" s="51" t="s">
+      <c r="CC2" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="CC2" s="51" t="s">
+      <c r="CD2" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="CD2" s="51" t="s">
+      <c r="CE2" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="CE2" s="51" t="s">
+      <c r="CF2" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="CF2" s="47"/>
+      <c r="CG2" s="47"/>
     </row>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <f t="shared" ref="A3:A29" si="0">COUNTIF(D3,"&lt;&gt;"&amp;"")+COUNTIF(BR3,"&lt;&gt;"&amp;"")</f>
         <v>1</v>
@@ -3157,15 +3183,18 @@
       <c r="BX3" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="BY3"/>
+      <c r="BY3" s="69">
+        <v>5</v>
+      </c>
       <c r="BZ3"/>
       <c r="CA3"/>
       <c r="CB3"/>
       <c r="CC3"/>
       <c r="CD3"/>
       <c r="CE3"/>
+      <c r="CF3"/>
     </row>
-    <row r="4" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3339,15 +3368,18 @@
       <c r="BX4" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="BY4"/>
+      <c r="BY4" s="69">
+        <v>5</v>
+      </c>
       <c r="BZ4"/>
       <c r="CA4"/>
       <c r="CB4"/>
       <c r="CC4"/>
       <c r="CD4"/>
       <c r="CE4"/>
+      <c r="CF4"/>
     </row>
-    <row r="5" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3521,15 +3553,18 @@
       <c r="BX5" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="BY5"/>
+      <c r="BY5" s="69">
+        <v>5</v>
+      </c>
       <c r="BZ5"/>
       <c r="CA5"/>
       <c r="CB5"/>
       <c r="CC5"/>
       <c r="CD5"/>
       <c r="CE5"/>
+      <c r="CF5"/>
     </row>
-    <row r="6" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3703,15 +3738,18 @@
       <c r="BX6" s="65" t="s">
         <v>364</v>
       </c>
-      <c r="BY6"/>
+      <c r="BY6" s="66">
+        <v>8</v>
+      </c>
       <c r="BZ6"/>
       <c r="CA6"/>
       <c r="CB6"/>
       <c r="CC6"/>
       <c r="CD6"/>
       <c r="CE6"/>
+      <c r="CF6"/>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3885,15 +3923,18 @@
       <c r="BX7" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY7"/>
+      <c r="BY7" s="66">
+        <v>8</v>
+      </c>
       <c r="BZ7"/>
       <c r="CA7"/>
       <c r="CB7"/>
       <c r="CC7"/>
       <c r="CD7"/>
       <c r="CE7"/>
+      <c r="CF7"/>
     </row>
-    <row r="8" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4067,15 +4108,18 @@
       <c r="BX8" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY8"/>
+      <c r="BY8" s="66">
+        <v>8</v>
+      </c>
       <c r="BZ8"/>
       <c r="CA8"/>
       <c r="CB8"/>
       <c r="CC8"/>
       <c r="CD8"/>
       <c r="CE8"/>
+      <c r="CF8"/>
     </row>
-    <row r="9" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4249,15 +4293,18 @@
       <c r="BX9" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY9"/>
+      <c r="BY9" s="66">
+        <v>20</v>
+      </c>
       <c r="BZ9"/>
       <c r="CA9"/>
       <c r="CB9"/>
       <c r="CC9"/>
       <c r="CD9"/>
       <c r="CE9"/>
+      <c r="CF9"/>
     </row>
-    <row r="10" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4431,15 +4478,18 @@
       <c r="BX10" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY10"/>
+      <c r="BY10" s="66">
+        <v>20</v>
+      </c>
       <c r="BZ10"/>
       <c r="CA10"/>
       <c r="CB10"/>
       <c r="CC10"/>
       <c r="CD10"/>
       <c r="CE10"/>
+      <c r="CF10"/>
     </row>
-    <row r="11" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4613,15 +4663,18 @@
       <c r="BX11" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY11"/>
+      <c r="BY11" s="66">
+        <v>20</v>
+      </c>
       <c r="BZ11"/>
       <c r="CA11"/>
       <c r="CB11"/>
       <c r="CC11"/>
       <c r="CD11"/>
       <c r="CE11"/>
+      <c r="CF11"/>
     </row>
-    <row r="12" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4795,15 +4848,18 @@
       <c r="BX12" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY12"/>
+      <c r="BY12" s="69">
+        <v>5</v>
+      </c>
       <c r="BZ12"/>
       <c r="CA12"/>
       <c r="CB12"/>
       <c r="CC12"/>
       <c r="CD12"/>
       <c r="CE12"/>
+      <c r="CF12"/>
     </row>
-    <row r="13" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4977,15 +5033,18 @@
       <c r="BX13" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY13"/>
+      <c r="BY13" s="69">
+        <v>5</v>
+      </c>
       <c r="BZ13"/>
       <c r="CA13"/>
       <c r="CB13"/>
       <c r="CC13"/>
       <c r="CD13"/>
       <c r="CE13"/>
+      <c r="CF13"/>
     </row>
-    <row r="14" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5159,15 +5218,18 @@
       <c r="BX14" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY14"/>
+      <c r="BY14" s="69">
+        <v>5</v>
+      </c>
       <c r="BZ14"/>
       <c r="CA14"/>
       <c r="CB14"/>
       <c r="CC14"/>
       <c r="CD14"/>
       <c r="CE14"/>
+      <c r="CF14"/>
     </row>
-    <row r="15" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5341,15 +5403,18 @@
       <c r="BX15" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY15"/>
+      <c r="BY15" s="66">
+        <v>8</v>
+      </c>
       <c r="BZ15"/>
       <c r="CA15"/>
       <c r="CB15"/>
       <c r="CC15"/>
       <c r="CD15"/>
       <c r="CE15"/>
+      <c r="CF15"/>
     </row>
-    <row r="16" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5513,15 +5578,18 @@
       <c r="BX16" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY16"/>
+      <c r="BY16" s="66">
+        <v>8</v>
+      </c>
       <c r="BZ16"/>
       <c r="CA16"/>
       <c r="CB16"/>
       <c r="CC16"/>
       <c r="CD16"/>
       <c r="CE16"/>
+      <c r="CF16"/>
     </row>
-    <row r="17" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5685,15 +5753,18 @@
       <c r="BX17" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY17"/>
+      <c r="BY17" s="66">
+        <v>8</v>
+      </c>
       <c r="BZ17"/>
       <c r="CA17"/>
       <c r="CB17"/>
       <c r="CC17"/>
       <c r="CD17"/>
       <c r="CE17"/>
+      <c r="CF17"/>
     </row>
-    <row r="18" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5857,15 +5928,18 @@
       <c r="BX18" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY18"/>
+      <c r="BY18" s="66">
+        <v>20</v>
+      </c>
       <c r="BZ18"/>
       <c r="CA18"/>
       <c r="CB18"/>
       <c r="CC18"/>
       <c r="CD18"/>
       <c r="CE18"/>
+      <c r="CF18"/>
     </row>
-    <row r="19" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6029,15 +6103,18 @@
       <c r="BX19" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY19"/>
+      <c r="BY19" s="66">
+        <v>20</v>
+      </c>
       <c r="BZ19"/>
       <c r="CA19"/>
       <c r="CB19"/>
       <c r="CC19"/>
       <c r="CD19"/>
       <c r="CE19"/>
+      <c r="CF19"/>
     </row>
-    <row r="20" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6201,15 +6278,18 @@
       <c r="BX20" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY20"/>
+      <c r="BY20" s="66">
+        <v>20</v>
+      </c>
       <c r="BZ20"/>
       <c r="CA20"/>
       <c r="CB20"/>
       <c r="CC20"/>
       <c r="CD20"/>
       <c r="CE20"/>
+      <c r="CF20"/>
     </row>
-    <row r="21" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6373,15 +6453,18 @@
       <c r="BX21" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="BY21"/>
+      <c r="BY21" s="69">
+        <v>5</v>
+      </c>
       <c r="BZ21"/>
       <c r="CA21"/>
       <c r="CB21"/>
       <c r="CC21"/>
       <c r="CD21"/>
       <c r="CE21"/>
+      <c r="CF21"/>
     </row>
-    <row r="22" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6545,15 +6628,18 @@
       <c r="BX22" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="BY22"/>
+      <c r="BY22" s="69">
+        <v>5</v>
+      </c>
       <c r="BZ22"/>
       <c r="CA22"/>
       <c r="CB22"/>
       <c r="CC22"/>
       <c r="CD22"/>
       <c r="CE22"/>
+      <c r="CF22"/>
     </row>
-    <row r="23" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6717,15 +6803,18 @@
       <c r="BX23" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="BY23"/>
+      <c r="BY23" s="69">
+        <v>5</v>
+      </c>
       <c r="BZ23"/>
       <c r="CA23"/>
       <c r="CB23"/>
       <c r="CC23"/>
       <c r="CD23"/>
       <c r="CE23"/>
+      <c r="CF23"/>
     </row>
-    <row r="24" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6889,15 +6978,18 @@
       <c r="BX24" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY24"/>
+      <c r="BY24" s="66">
+        <v>8</v>
+      </c>
       <c r="BZ24"/>
       <c r="CA24"/>
       <c r="CB24"/>
       <c r="CC24"/>
       <c r="CD24"/>
       <c r="CE24"/>
+      <c r="CF24"/>
     </row>
-    <row r="25" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7061,15 +7153,18 @@
       <c r="BX25" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY25"/>
+      <c r="BY25" s="66">
+        <v>8</v>
+      </c>
       <c r="BZ25"/>
       <c r="CA25"/>
       <c r="CB25"/>
       <c r="CC25"/>
       <c r="CD25"/>
       <c r="CE25"/>
+      <c r="CF25"/>
     </row>
-    <row r="26" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7233,15 +7328,18 @@
       <c r="BX26" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY26"/>
+      <c r="BY26" s="66">
+        <v>8</v>
+      </c>
       <c r="BZ26"/>
       <c r="CA26"/>
       <c r="CB26"/>
       <c r="CC26"/>
       <c r="CD26"/>
       <c r="CE26"/>
+      <c r="CF26"/>
     </row>
-    <row r="27" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A27" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7405,15 +7503,18 @@
       <c r="BX27" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY27"/>
+      <c r="BY27" s="66">
+        <v>20</v>
+      </c>
       <c r="BZ27"/>
       <c r="CA27"/>
       <c r="CB27"/>
       <c r="CC27"/>
       <c r="CD27"/>
       <c r="CE27"/>
+      <c r="CF27"/>
     </row>
-    <row r="28" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A28" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7577,15 +7678,18 @@
       <c r="BX28" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY28"/>
+      <c r="BY28" s="66">
+        <v>20</v>
+      </c>
       <c r="BZ28"/>
       <c r="CA28"/>
       <c r="CB28"/>
       <c r="CC28"/>
       <c r="CD28"/>
       <c r="CE28"/>
+      <c r="CF28"/>
     </row>
-    <row r="29" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A29" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7749,21 +7853,24 @@
       <c r="BX29" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY29"/>
+      <c r="BY29" s="66">
+        <v>20</v>
+      </c>
       <c r="BZ29"/>
       <c r="CA29"/>
       <c r="CB29"/>
       <c r="CC29"/>
       <c r="CD29"/>
       <c r="CE29"/>
+      <c r="CF29"/>
     </row>
-    <row r="30" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:84" x14ac:dyDescent="0.2">
       <c r="AO30" s="13"/>
     </row>
-    <row r="31" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:84" x14ac:dyDescent="0.2">
       <c r="AO31" s="13"/>
     </row>
-    <row r="32" spans="1:83" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:84" x14ac:dyDescent="0.2">
       <c r="AO32" s="13"/>
     </row>
     <row r="33" spans="41:41" x14ac:dyDescent="0.2">
@@ -7825,9 +7932,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -7845,24 +7962,14 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Update distance to exhaust
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/sinclair/testproj/metadata.xlsx
+++ b/metadata/excel/projects/sinclair/testproj/metadata.xlsx
@@ -16,10 +16,10 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -1911,13 +1911,13 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2609,7 +2609,7 @@
     <sheetView tabSelected="1" topLeftCell="BK1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="BZ7" sqref="BZ7"/>
+      <selection pane="bottomLeft" activeCell="CA5" sqref="CA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2746,25 +2746,25 @@
       <c r="BC1" s="3"/>
       <c r="BD1" s="3"/>
       <c r="BE1" s="10"/>
-      <c r="BG1" s="67" t="s">
+      <c r="BG1" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="BH1" s="67"/>
-      <c r="BI1" s="67"/>
-      <c r="BJ1" s="67"/>
-      <c r="BL1" s="67" t="s">
+      <c r="BH1" s="69"/>
+      <c r="BI1" s="69"/>
+      <c r="BJ1" s="69"/>
+      <c r="BL1" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="BM1" s="67"/>
-      <c r="BN1" s="67"/>
-      <c r="BO1" s="67"/>
-      <c r="BP1" s="67"/>
-      <c r="BQ1" s="67"/>
-      <c r="BR1" s="67"/>
-      <c r="BT1" s="67" t="s">
+      <c r="BM1" s="69"/>
+      <c r="BN1" s="69"/>
+      <c r="BO1" s="69"/>
+      <c r="BP1" s="69"/>
+      <c r="BQ1" s="69"/>
+      <c r="BR1" s="69"/>
+      <c r="BT1" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="BU1" s="67"/>
+      <c r="BU1" s="69"/>
       <c r="BW1" s="8" t="s">
         <v>68</v>
       </c>
@@ -2983,7 +2983,7 @@
       <c r="BX2" s="51" t="s">
         <v>362</v>
       </c>
-      <c r="BY2" s="68" t="s">
+      <c r="BY2" s="67" t="s">
         <v>365</v>
       </c>
       <c r="BZ2" s="51" t="s">
@@ -3183,8 +3183,8 @@
       <c r="BX3" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="BY3" s="69">
-        <v>5</v>
+      <c r="BY3" s="68">
+        <v>0</v>
       </c>
       <c r="BZ3"/>
       <c r="CA3"/>
@@ -3368,8 +3368,8 @@
       <c r="BX4" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="BY4" s="69">
-        <v>5</v>
+      <c r="BY4" s="68">
+        <v>0</v>
       </c>
       <c r="BZ4"/>
       <c r="CA4"/>
@@ -3553,8 +3553,8 @@
       <c r="BX5" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="BY5" s="69">
-        <v>5</v>
+      <c r="BY5" s="68">
+        <v>0</v>
       </c>
       <c r="BZ5"/>
       <c r="CA5"/>
@@ -3739,7 +3739,7 @@
         <v>364</v>
       </c>
       <c r="BY6" s="66">
-        <v>8</v>
+        <v>545.16</v>
       </c>
       <c r="BZ6"/>
       <c r="CA6"/>
@@ -3924,7 +3924,7 @@
         <v>364</v>
       </c>
       <c r="BY7" s="66">
-        <v>8</v>
+        <v>545.16</v>
       </c>
       <c r="BZ7"/>
       <c r="CA7"/>
@@ -4109,7 +4109,7 @@
         <v>364</v>
       </c>
       <c r="BY8" s="66">
-        <v>8</v>
+        <v>545.16</v>
       </c>
       <c r="BZ8"/>
       <c r="CA8"/>
@@ -4294,7 +4294,7 @@
         <v>364</v>
       </c>
       <c r="BY9" s="66">
-        <v>20</v>
+        <v>5080.2700000000004</v>
       </c>
       <c r="BZ9"/>
       <c r="CA9"/>
@@ -4479,7 +4479,7 @@
         <v>364</v>
       </c>
       <c r="BY10" s="66">
-        <v>20</v>
+        <v>5080.2700000000004</v>
       </c>
       <c r="BZ10"/>
       <c r="CA10"/>
@@ -4664,7 +4664,7 @@
         <v>364</v>
       </c>
       <c r="BY11" s="66">
-        <v>20</v>
+        <v>5080.2700000000004</v>
       </c>
       <c r="BZ11"/>
       <c r="CA11"/>
@@ -4848,8 +4848,8 @@
       <c r="BX12" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY12" s="69">
-        <v>5</v>
+      <c r="BY12" s="68">
+        <v>0</v>
       </c>
       <c r="BZ12"/>
       <c r="CA12"/>
@@ -5033,8 +5033,8 @@
       <c r="BX13" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY13" s="69">
-        <v>5</v>
+      <c r="BY13" s="68">
+        <v>0</v>
       </c>
       <c r="BZ13"/>
       <c r="CA13"/>
@@ -5218,8 +5218,8 @@
       <c r="BX14" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="BY14" s="69">
-        <v>5</v>
+      <c r="BY14" s="68">
+        <v>0</v>
       </c>
       <c r="BZ14"/>
       <c r="CA14"/>
@@ -5404,7 +5404,7 @@
         <v>364</v>
       </c>
       <c r="BY15" s="66">
-        <v>8</v>
+        <v>175.69</v>
       </c>
       <c r="BZ15"/>
       <c r="CA15"/>
@@ -5579,7 +5579,7 @@
         <v>364</v>
       </c>
       <c r="BY16" s="66">
-        <v>8</v>
+        <v>175.69</v>
       </c>
       <c r="BZ16"/>
       <c r="CA16"/>
@@ -5754,7 +5754,7 @@
         <v>364</v>
       </c>
       <c r="BY17" s="66">
-        <v>8</v>
+        <v>175.69</v>
       </c>
       <c r="BZ17"/>
       <c r="CA17"/>
@@ -5929,7 +5929,7 @@
         <v>364</v>
       </c>
       <c r="BY18" s="66">
-        <v>20</v>
+        <v>1235.56</v>
       </c>
       <c r="BZ18"/>
       <c r="CA18"/>
@@ -6104,7 +6104,7 @@
         <v>364</v>
       </c>
       <c r="BY19" s="66">
-        <v>20</v>
+        <v>1235.56</v>
       </c>
       <c r="BZ19"/>
       <c r="CA19"/>
@@ -6279,7 +6279,7 @@
         <v>364</v>
       </c>
       <c r="BY20" s="66">
-        <v>20</v>
+        <v>1235.56</v>
       </c>
       <c r="BZ20"/>
       <c r="CA20"/>
@@ -6453,8 +6453,8 @@
       <c r="BX21" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="BY21" s="69">
-        <v>5</v>
+      <c r="BY21" s="68">
+        <v>0</v>
       </c>
       <c r="BZ21"/>
       <c r="CA21"/>
@@ -6628,8 +6628,8 @@
       <c r="BX22" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="BY22" s="69">
-        <v>5</v>
+      <c r="BY22" s="68">
+        <v>0</v>
       </c>
       <c r="BZ22"/>
       <c r="CA22"/>
@@ -6803,8 +6803,8 @@
       <c r="BX23" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="BY23" s="69">
-        <v>5</v>
+      <c r="BY23" s="68">
+        <v>0</v>
       </c>
       <c r="BZ23"/>
       <c r="CA23"/>
@@ -6979,7 +6979,7 @@
         <v>364</v>
       </c>
       <c r="BY24" s="66">
-        <v>8</v>
+        <v>338.21</v>
       </c>
       <c r="BZ24"/>
       <c r="CA24"/>
@@ -7154,7 +7154,7 @@
         <v>364</v>
       </c>
       <c r="BY25" s="66">
-        <v>8</v>
+        <v>338.21</v>
       </c>
       <c r="BZ25"/>
       <c r="CA25"/>
@@ -7329,7 +7329,7 @@
         <v>364</v>
       </c>
       <c r="BY26" s="66">
-        <v>8</v>
+        <v>338.21</v>
       </c>
       <c r="BZ26"/>
       <c r="CA26"/>
@@ -7504,7 +7504,7 @@
         <v>364</v>
       </c>
       <c r="BY27" s="66">
-        <v>20</v>
+        <v>4192.68</v>
       </c>
       <c r="BZ27"/>
       <c r="CA27"/>
@@ -7679,7 +7679,7 @@
         <v>364</v>
       </c>
       <c r="BY28" s="66">
-        <v>20</v>
+        <v>4192.68</v>
       </c>
       <c r="BZ28"/>
       <c r="CA28"/>
@@ -7854,7 +7854,7 @@
         <v>364</v>
       </c>
       <c r="BY29" s="66">
-        <v>20</v>
+        <v>4192.68</v>
       </c>
       <c r="BZ29"/>
       <c r="CA29"/>
@@ -7932,19 +7932,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -7962,14 +7952,24 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Small mitake in label numbers
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/sinclair/testproj/metadata.xlsx
+++ b/metadata/excel/projects/sinclair/testproj/metadata.xlsx
@@ -16,10 +16,10 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="391">
   <si>
     <t>Country</t>
   </si>
@@ -1225,6 +1225,12 @@
   </si>
   <si>
     <t>HA dist 3</t>
+  </si>
+  <si>
+    <t>AS dist 2</t>
+  </si>
+  <si>
+    <t>AS dist 3</t>
   </si>
 </sst>
 </file>
@@ -2588,7 +2594,7 @@
     <sheetView tabSelected="1" topLeftCell="P1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="AD45" sqref="AD44:AD45"/>
+      <selection pane="bottomLeft" activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2755,7 +2761,7 @@
       <c r="CC1" s="21"/>
       <c r="CD1" s="21"/>
     </row>
-    <row r="2" spans="1:83" s="52" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:83" s="52" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
         <v>46</v>
       </c>
@@ -4393,7 +4399,7 @@
         <v>3</v>
       </c>
       <c r="Z10" s="32" t="s">
-        <v>370</v>
+        <v>389</v>
       </c>
       <c r="AA10" s="1"/>
       <c r="AB10" s="32" t="s">
@@ -4586,7 +4592,7 @@
         <v>3</v>
       </c>
       <c r="Z11" s="32" t="s">
-        <v>370</v>
+        <v>390</v>
       </c>
       <c r="AA11" s="1"/>
       <c r="AB11" s="32" t="s">
@@ -8119,9 +8125,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -8139,24 +8155,14 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Update exhaust pipe distances, step 2
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/sinclair/testproj/metadata.xlsx
+++ b/metadata/excel/projects/sinclair/testproj/metadata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,22 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12040" yWindow="5160" windowWidth="36620" windowHeight="22320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51120" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="micans_v6_ex1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1754,7 +1751,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1903,6 +1900,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2591,10 +2591,10 @@
   </sheetPr>
   <dimension ref="A1:CE51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BS1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="AA7" sqref="AA7"/>
+      <selection pane="bottomLeft" activeCell="CG15" sqref="CG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3163,8 +3163,8 @@
       <c r="BY3" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="BZ3" s="41">
-        <v>0</v>
+      <c r="BZ3" s="70">
+        <v>154.41999999999999</v>
       </c>
       <c r="CA3">
         <v>42.3</v>
@@ -3356,8 +3356,8 @@
       <c r="BY4" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="BZ4" s="41">
-        <v>0</v>
+      <c r="BZ4" s="70">
+        <v>154.41999999999999</v>
       </c>
       <c r="CA4">
         <v>42.3</v>
@@ -3549,8 +3549,8 @@
       <c r="BY5" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="BZ5" s="41">
-        <v>0</v>
+      <c r="BZ5" s="70">
+        <v>154.41999999999999</v>
       </c>
       <c r="CA5">
         <v>42.3</v>
@@ -3742,8 +3742,8 @@
       <c r="BY6" s="65" t="s">
         <v>358</v>
       </c>
-      <c r="BZ6" s="65">
-        <v>545.16</v>
+      <c r="BZ6" s="66">
+        <v>694.57</v>
       </c>
       <c r="CA6">
         <v>39.6</v>
@@ -3936,7 +3936,7 @@
         <v>358</v>
       </c>
       <c r="BZ7" s="66">
-        <v>545.16</v>
+        <v>694.57</v>
       </c>
       <c r="CA7">
         <v>39.6</v>
@@ -4129,7 +4129,7 @@
         <v>358</v>
       </c>
       <c r="BZ8" s="66">
-        <v>545.16</v>
+        <v>694.57</v>
       </c>
       <c r="CA8">
         <v>39.6</v>
@@ -4322,7 +4322,7 @@
         <v>358</v>
       </c>
       <c r="BZ9" s="66">
-        <v>5080.2700000000004</v>
+        <v>5022.16</v>
       </c>
       <c r="CA9">
         <v>39.6</v>
@@ -4515,7 +4515,7 @@
         <v>358</v>
       </c>
       <c r="BZ10" s="66">
-        <v>5080.2700000000004</v>
+        <v>5022.16</v>
       </c>
       <c r="CA10">
         <v>39.6</v>
@@ -4708,7 +4708,7 @@
         <v>358</v>
       </c>
       <c r="BZ11" s="66">
-        <v>5080.2700000000004</v>
+        <v>5022.16</v>
       </c>
       <c r="CA11">
         <v>39.6</v>
@@ -4900,7 +4900,7 @@
       <c r="BY12" s="66" t="s">
         <v>358</v>
       </c>
-      <c r="BZ12" s="41">
+      <c r="BZ12" s="70">
         <v>102.78</v>
       </c>
       <c r="CA12">
@@ -5093,7 +5093,7 @@
       <c r="BY13" s="66" t="s">
         <v>358</v>
       </c>
-      <c r="BZ13" s="41">
+      <c r="BZ13" s="70">
         <v>102.78</v>
       </c>
       <c r="CA13">
@@ -5286,7 +5286,7 @@
       <c r="BY14" s="66" t="s">
         <v>358</v>
       </c>
-      <c r="BZ14" s="41">
+      <c r="BZ14" s="70">
         <v>102.78</v>
       </c>
       <c r="CA14">
@@ -5479,7 +5479,7 @@
       <c r="BY15" s="66" t="s">
         <v>358</v>
       </c>
-      <c r="BZ15" s="65">
+      <c r="BZ15" s="66">
         <v>130.54</v>
       </c>
       <c r="CA15">
@@ -6577,8 +6577,8 @@
       <c r="BY21" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="BZ21" s="41">
-        <v>0</v>
+      <c r="BZ21" s="70">
+        <v>118.45</v>
       </c>
       <c r="CA21">
         <v>41.04</v>
@@ -6760,8 +6760,8 @@
       <c r="BY22" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="BZ22" s="41">
-        <v>0</v>
+      <c r="BZ22" s="70">
+        <v>118.45</v>
       </c>
       <c r="CA22">
         <v>41.04</v>
@@ -6943,8 +6943,8 @@
       <c r="BY23" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="BZ23" s="41">
-        <v>0</v>
+      <c r="BZ23" s="70">
+        <v>118.45</v>
       </c>
       <c r="CA23">
         <v>41.04</v>
@@ -7126,8 +7126,8 @@
       <c r="BY24" s="66" t="s">
         <v>358</v>
       </c>
-      <c r="BZ24" s="65">
-        <v>338.21</v>
+      <c r="BZ24" s="66">
+        <v>454.75</v>
       </c>
       <c r="CA24">
         <v>39.4</v>
@@ -7310,7 +7310,7 @@
         <v>358</v>
       </c>
       <c r="BZ25" s="66">
-        <v>338.21</v>
+        <v>454.75</v>
       </c>
       <c r="CA25">
         <v>39.4</v>
@@ -7493,7 +7493,7 @@
         <v>358</v>
       </c>
       <c r="BZ26" s="66">
-        <v>338.21</v>
+        <v>454.75</v>
       </c>
       <c r="CA26">
         <v>39.4</v>
@@ -7676,7 +7676,7 @@
         <v>358</v>
       </c>
       <c r="BZ27" s="66">
-        <v>4192.68</v>
+        <v>4288.6400000000003</v>
       </c>
       <c r="CA27">
         <v>39.5</v>
@@ -7859,7 +7859,7 @@
         <v>358</v>
       </c>
       <c r="BZ28" s="66">
-        <v>4192.68</v>
+        <v>4288.6400000000003</v>
       </c>
       <c r="CA28">
         <v>39.5</v>
@@ -8042,7 +8042,7 @@
         <v>358</v>
       </c>
       <c r="BZ29" s="66">
-        <v>4192.68</v>
+        <v>4288.6400000000003</v>
       </c>
       <c r="CA29">
         <v>39.5</v>
@@ -8125,19 +8125,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -8155,14 +8145,24 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>